<commit_message>
Auto-committed on 2022/01/12 週三
Former-commit-id: 86c1be4cea70565c5e59837669865e8f83f8cad0
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L3-帳務作業/LoanBorMain.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L3-帳務作業/LoanBorMain.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L3-帳務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968EBA09-BBC4-4D68-BA79-F26BCCFF4B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE17A40-AD8A-49AD-A154-6965D32DFA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1784,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2977,7 +2977,7 @@
         <v>112</v>
       </c>
       <c r="E59" s="12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F59" s="12"/>
       <c r="G59" s="25"/>

</xml_diff>